<commit_message>
rearranged background & some more verification
</commit_message>
<xml_diff>
--- a/s2n-harness/unit/testReport.xlsx
+++ b/s2n-harness/unit/testReport.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="-20" yWindow="0" windowWidth="29940" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>s2n_3des_harness</t>
   </si>
@@ -112,9 +112,6 @@
   </si>
   <si>
     <t>s2n_tls_record_stuffer_harness</t>
-  </si>
-  <si>
-    <t xml:space="preserve">       s</t>
   </si>
   <si>
     <t>Harness</t>
@@ -559,10 +556,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -575,44 +572,44 @@
     <col min="6" max="6" width="20.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="23" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="93" customWidth="1"/>
+    <col min="9" max="9" width="162.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="135">
+    </row>
+    <row r="2" spans="1:9" ht="75">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -755,10 +752,10 @@
         <v>28</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -771,14 +768,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
-      <c r="A33" t="s">
-        <v>31</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>